<commit_message>
A spiral iterator that's not evenly-spaced
</commit_message>
<xml_diff>
--- a/eg/Test Case.xlsx
+++ b/eg/Test Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -478,7 +478,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,7 +497,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="J1" t="s">
         <v>1</v>
       </c>
@@ -507,10 +509,14 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -546,7 +552,9 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" t="s">
@@ -581,7 +589,9 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>

</xml_diff>

<commit_message>
Getting the basic case working
</commit_message>
<xml_diff>
--- a/eg/Test Case.xlsx
+++ b/eg/Test Case.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
-  <si>
-    <t>x</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Center X</t>
   </si>
@@ -475,159 +472,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="3.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="10"/>
+    <col min="2" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="10">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="10">
+      <c r="L2" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="K2" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="K3" s="10">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5">
+        <v>13</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-      <c r="J4" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="K4" s="10">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="K5" s="10">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="D7" s="5">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5">
+        <v>10</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+      <c r="D8" s="5">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5">
+        <v>23</v>
+      </c>
+      <c r="G8" s="5">
+        <v>24</v>
+      </c>
+      <c r="H8" s="5">
+        <v>25</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>